<commit_message>
moved metadata in ID Sawtooth data
</commit_message>
<xml_diff>
--- a/data/raw/USFWS_bull_trout_SSA_data_ID_Sawtooth.xlsx
+++ b/data/raw/USFWS_bull_trout_SSA_data_ID_Sawtooth.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008C289B-2581-E441-8240-EC1C4D779F2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F466CE-29F8-1D48-A542-DDCA2504FD7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11400" yWindow="5060" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ID data" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="15">
   <si>
     <t>recovery unit</t>
   </si>
@@ -63,13 +64,13 @@
     <t>Weir</t>
   </si>
   <si>
-    <t>MetaData</t>
-  </si>
-  <si>
     <t>Hatchery weir operated at Sawtooth Fish Hatchery. Weir is operated to collect spring/summer Chinook for the hatchery program. However, BT are caught at the facility. Operations have been consistent across the dataseries.</t>
   </si>
   <si>
     <t>dataset</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -396,11 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -413,7 +412,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -749,12 +748,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E570D2-6444-CB45-B0A4-A12C08C4640C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>